<commit_message>
Template MBKM V.1 (Sebelum ada masukan)
</commit_message>
<xml_diff>
--- a/public/document/template_nilai.xlsx
+++ b/public/document/template_nilai.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/HDD/2021/ASDOS/MBKM Analys/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Library/WebServer/Documents/www/MYMBKM/public/document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0183A5D-B16F-584C-985D-FD3A210ADB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B29F97-A7C8-E741-9C43-FE3BF7D8538A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="1" xr2:uid="{645B4DD9-B053-E44C-A11B-162A02249FBC}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{645B4DD9-B053-E44C-A11B-162A02249FBC}"/>
   </bookViews>
   <sheets>
     <sheet name="MK1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>PEMBIMBING</t>
   </si>
   <si>
-    <t>Diah Priyawati, S.T, M.Eng</t>
-  </si>
-  <si>
     <t>SKS</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>SETIAWAN</t>
+  </si>
+  <si>
+    <t>Ir. Purwo Setiawan, Ph.D</t>
   </si>
 </sst>
 </file>
@@ -229,12 +229,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -245,6 +239,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBEECF48-C14B-AD4D-A6FE-7689C8AB656D}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,35 +683,35 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="11" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -721,7 +721,7 @@
         <v>4</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I8" s="1">
         <v>3</v>
@@ -735,7 +735,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" s="1">
         <v>7</v>
@@ -752,89 +752,89 @@
         <v>10</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="J12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K12" s="4" t="s">
+      <c r="E13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="5">
+        <v>1</v>
+      </c>
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>1</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="7">
-        <v>1</v>
-      </c>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
-        <v>1</v>
-      </c>
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -854,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DF66C6-5A1E-234C-8D60-4163EABA436D}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -888,35 +888,35 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="11" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -926,7 +926,7 @@
         <v>4</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I8" s="1">
         <v>3</v>
@@ -940,7 +940,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" s="1">
         <v>7</v>
@@ -957,89 +957,89 @@
         <v>10</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="J12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K12" s="4" t="s">
+      <c r="E13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="5">
+        <v>1</v>
+      </c>
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>1</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="7">
-        <v>1</v>
-      </c>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
-        <v>1</v>
-      </c>
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>